<commit_message>
Made delete work and started on sorts
</commit_message>
<xml_diff>
--- a/TestUser.xlsx
+++ b/TestUser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,76 +434,170 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="E1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="F1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="G1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="H1" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Test Transaction</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="D2" t="n">
+        <v>5</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>Transaction 1</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Test Transaction 2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>Transaction 5</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>500</v>
+      </c>
+      <c r="G3" t="n">
+        <v>50</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>Transaction 4</t>
         </is>
+      </c>
+      <c r="F4" t="n">
+        <v>400</v>
+      </c>
+      <c r="G4" t="n">
+        <v>40</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Transaction 3</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>300</v>
+      </c>
+      <c r="G5" t="n">
+        <v>30</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Transaction 2</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>200</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed statistics and frames sizing
</commit_message>
<xml_diff>
--- a/TestUser.xlsx
+++ b/TestUser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,27 +436,22 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.1</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
+      <c r="C1" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="D1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -465,139 +460,26 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
-          <t>Transaction 1</t>
+          <t>Direct Deposit</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>5000</v>
+      </c>
       <c r="F2" t="n">
-        <v>100</v>
-      </c>
-      <c r="G2" t="n">
-        <v>10</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
-          <t>Transaction 5</t>
+          <t>1/13/2025</t>
         </is>
-      </c>
-      <c r="F3" t="n">
-        <v>500</v>
-      </c>
-      <c r="G3" t="n">
-        <v>50</v>
-      </c>
-      <c r="H3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Transaction 4</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>400</v>
-      </c>
-      <c r="G4" t="n">
-        <v>40</v>
-      </c>
-      <c r="H4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Transaction 3</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>300</v>
-      </c>
-      <c r="G5" t="n">
-        <v>30</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Transaction 2</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>200</v>
-      </c>
-      <c r="G6" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
styled the sign in menu
</commit_message>
<xml_diff>
--- a/TestUser.xlsx
+++ b/TestUser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,32 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="E1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="F1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="G1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="H1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="I1" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -460,25 +470,60 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Direct Deposit</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>5000</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>1/13/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Housing Purchase</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1/12/2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Create Accounts in Excel
</commit_message>
<xml_diff>
--- a/TestUser.xlsx
+++ b/TestUser.xlsx
@@ -1,37 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graha\Documents\GitHub\WP_Coding_And_Programming\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4D11A1-CAB7-44A4-847F-2670A181EFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="4350" yWindow="1995" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Direct Deposit</t>
+  </si>
+  <si>
+    <t>1/13/2025</t>
+  </si>
+  <si>
+    <t>Housing Purchase</t>
+  </si>
+  <si>
+    <t>1/12/2025</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +69,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,111 +393,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.2</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.1</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2">
+        <v>5000</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Direct Deposit</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1/13/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Housing Purchase</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="D3">
         <v>100000</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1/12/2025</t>
-        </is>
+      <c r="E3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to fix error
</commit_message>
<xml_diff>
--- a/TestUser.xlsx
+++ b/TestUser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graha\Documents\GitHub\WP_Coding_And_Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4D11A1-CAB7-44A4-847F-2670A181EFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3BAD5D-E0DD-4FFD-B62A-6DB2B584FE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4350" yWindow="1995" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,18 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Direct Deposit</t>
-  </si>
-  <si>
-    <t>1/13/2025</t>
-  </si>
-  <si>
-    <t>Housing Purchase</t>
-  </si>
-  <si>
-    <t>1/12/2025</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Mortage</t>
+  </si>
+  <si>
+    <t>01/01/2000</t>
+  </si>
+  <si>
+    <t>Paycheck</t>
+  </si>
+  <si>
+    <t>01/02/2000</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>01/03/2000</t>
+  </si>
+  <si>
+    <t>Dog Food</t>
+  </si>
+  <si>
+    <t>01/04/2000</t>
   </si>
 </sst>
 </file>
@@ -394,18 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -418,39 +427,88 @@
       <c r="E1" s="1">
         <v>4</v>
       </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>5000</v>
+      <c r="C2" t="s">
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="D3">
+        <v>5000</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>100000</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed signin breaking, stylized home_frame, added cumulative earnings to statistics_frame
</commit_message>
<xml_diff>
--- a/TestUser.xlsx
+++ b/TestUser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,94 +436,105 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.3</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0.2</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0.1</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="F1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="H1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="I1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="J1" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Direct Deposit</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>5000</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Housing Purchase</t>
+        </is>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1/13/2025</t>
+      <c r="I2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>1/12/2025</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Housing Purchase</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Direct Deposit</t>
+        </is>
       </c>
       <c r="H3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1/12/2025</t>
+        <v>5000</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1/13/2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added images for help
</commit_message>
<xml_diff>
--- a/TestUser.xlsx
+++ b/TestUser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,26 +436,28 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.4</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0.3</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0.2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0.1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0</t>
         </is>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>0</v>
       </c>
       <c r="G1" s="1" t="n">
         <v>1</v>
@@ -472,19 +474,19 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
         <v>2</v>
       </c>
-      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>2</v>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>Housing Purchase</t>
@@ -504,7 +506,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -516,7 +518,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -535,6 +537,32 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>1/13/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Pay from Work</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>1/14/2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
commits for database and flask server
</commit_message>
<xml_diff>
--- a/TestUser.xlsx
+++ b/TestUser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,91 +434,628 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="G1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="H1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="I1" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Housing Purchase</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>100000</v>
+        <v>7</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1/12/2025</t>
+          <t>Investment</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>300</v>
+      </c>
+      <c r="H2" t="n">
+        <v>200</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>5/4/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Direct Deposit</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
       </c>
       <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Housing Deposit</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>5000</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1/13/2025</t>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1/29/2024</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>300</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2/18/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c r="E5" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Pay from Work</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Paycheck</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2/20/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Volunteering</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>200</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3/8/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Mortgage</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3/16/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Loan to Friend</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>100</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>4/17/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>150</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>6/4/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Mortgage</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>7/5/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Paycheck</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>500</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>9/02/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Eating Out</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>200</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>11/15/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>12/1/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="n">
+        <v>13</v>
+      </c>
+      <c r="E14" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Lawnmowing</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>25</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>12/28/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n">
+        <v>14</v>
+      </c>
+      <c r="E15" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Oil Change</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>60</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1/2/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>15</v>
+      </c>
+      <c r="E16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Laptop Purchase</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1/4/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>16</v>
+      </c>
+      <c r="E17" t="n">
+        <v>16</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>150</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1/8/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>17</v>
+      </c>
+      <c r="E18" t="n">
+        <v>17</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>25</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1/11/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>18</v>
+      </c>
+      <c r="E19" t="n">
+        <v>18</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Paycheck</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
         <v>1500</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1/14/2025</t>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1/12/2025</t>
         </is>
       </c>
     </row>

</xml_diff>